<commit_message>
Update jadwal kuliah dan nambah materi
</commit_message>
<xml_diff>
--- a/Jadwal Kuliah.xlsx
+++ b/Jadwal Kuliah.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Zefanya\Dokumen\Kuliah\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A08457-02BA-47ED-A0A9-DF279C6262B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F81052-2637-4E63-B5E6-D4922D2611D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{E5D4EB63-BC32-484D-AEFA-16FF28B60A9B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Senin</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Praktikum Jarkom                                              08.00 - 09.40 (LIK)</t>
-  </si>
-  <si>
-    <t>Aslab - Praktikum PBO                                              09.50 - 11.30 (LIK)</t>
   </si>
 </sst>
 </file>
@@ -795,7 +792,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -856,7 +853,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Update Jadwal + Modul Praktikum
</commit_message>
<xml_diff>
--- a/Jadwal Kuliah.xlsx
+++ b/Jadwal Kuliah.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Zefanya\Dokumen\Kuliah\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B04281-4C93-4BB6-AF39-2DCB7D611E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFB93F5-7BAE-4734-8F7C-5094267FB363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{E5D4EB63-BC32-484D-AEFA-16FF28B60A9B}"/>
   </bookViews>
@@ -105,7 +105,7 @@
     <t>Praktikum Jarkom                                              08.00 - 09.40 (LIK)</t>
   </si>
   <si>
-    <t>AI                                               13.30 - 15.10 (D7)</t>
+    <t>AI                                               08.00 - 09.40 (D7)</t>
   </si>
 </sst>
 </file>
@@ -121,7 +121,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +164,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -418,9 +424,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -474,6 +477,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -792,7 +798,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -810,37 +816,37 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -849,43 +855,43 @@
       <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="28" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="20"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="2:10" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
     </row>
     <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E7" s="1"/>
@@ -896,7 +902,7 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1"/>
@@ -907,7 +913,7 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="1"/>
@@ -918,22 +924,22 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new files to Modul1 and Modul3 playground
</commit_message>
<xml_diff>
--- a/Jadwal Kuliah.xlsx
+++ b/Jadwal Kuliah.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Zefanya\Dokumen\Kuliah\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956CF5C1-50A5-49A5-AFAC-ABC660411923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361BD04C-B992-40DF-8224-B9C790DC382B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{E5D4EB63-BC32-484D-AEFA-16FF28B60A9B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{E5D4EB63-BC32-484D-AEFA-16FF28B60A9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Semester 4" sheetId="1" r:id="rId1"/>
+    <sheet name="Semester 5" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
   <si>
     <t>Senin</t>
   </si>
@@ -214,6 +215,36 @@
   </si>
   <si>
     <t>Pemrograman Game (13.35 - 16.00 || G9)</t>
+  </si>
+  <si>
+    <t>Aslab - Praktikum PD                                              13:00-16:00 (LIK)</t>
+  </si>
+  <si>
+    <t>Stupen - MAD LearningX                                      14:00 - Selesai (Zoom)</t>
+  </si>
+  <si>
+    <t>Stupen - MAD LearningX                                      08:30 - Selesai (Zoom)</t>
+  </si>
+  <si>
+    <t>Aslab - Praktikum Database  A                                         10.40 - 12.40 (LIK)</t>
+  </si>
+  <si>
+    <t>Aslab - Praktikum SO A                                             10.40 - 12.40 (LIK)</t>
+  </si>
+  <si>
+    <t>Aslab - Praktikum SO B                                             10.40 - 12.40 (LIK)</t>
+  </si>
+  <si>
+    <t>PBW Lanjut                                09:50 - 11:30 (E10)</t>
+  </si>
+  <si>
+    <t>Aslab - Praktikum PBW A                                             08.00 - 10.30 (LIK)</t>
+  </si>
+  <si>
+    <t>Jadwal Kuliah Semester 5</t>
+  </si>
+  <si>
+    <t>Stupen - MAD LearningX                                            ?? - ??  (Zoom)</t>
   </si>
 </sst>
 </file>
@@ -291,7 +322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -592,11 +623,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -619,7 +738,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -679,6 +797,24 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -702,6 +838,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1263,8 +1408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A500BB-88A3-46AD-8552-90057F608116}">
   <dimension ref="B1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="102" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView zoomScale="102" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1281,14 +1426,14 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="36"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="43"/>
     </row>
     <row r="3" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
@@ -1306,12 +1451,12 @@
       <c r="F3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1320,43 +1465,43 @@
       <c r="D4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="19"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="2:10" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E7" s="1"/>
@@ -1367,7 +1512,7 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1"/>
@@ -1399,157 +1544,157 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="35" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="25" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="27" t="s">
+      <c r="H17" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="27" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="I20" s="31" t="s">
+      <c r="I20" s="30" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F21" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="G21" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H21" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="I21" s="27" t="s">
+      <c r="I21" s="26" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="32"/>
-      <c r="C22" s="28" t="s">
+      <c r="B22" s="31"/>
+      <c r="C22" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="28" t="s">
+      <c r="D22" s="32"/>
+      <c r="E22" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="39"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="41"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1561,4 +1706,130 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554D7EEC-089B-442B-85F1-238477FC9684}">
+  <dimension ref="C1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="29.08984375" customWidth="1"/>
+    <col min="4" max="4" width="31.90625" customWidth="1"/>
+    <col min="5" max="5" width="33.08984375" customWidth="1"/>
+    <col min="6" max="6" width="26.6328125" customWidth="1"/>
+    <col min="7" max="7" width="24.7265625" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51"/>
+    </row>
+    <row r="3" spans="3:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="43" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="38"/>
+      <c r="G5" s="36"/>
+    </row>
+    <row r="6" spans="3:7" ht="53.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="40"/>
+      <c r="E6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="37"/>
+    </row>
+    <row r="7" spans="3:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E7" s="34"/>
+    </row>
+    <row r="8" spans="3:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C9" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C10" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C13" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove unused test file, update import paths, and add launch configuration for Dart & Flutter
</commit_message>
<xml_diff>
--- a/Jadwal Kuliah.xlsx
+++ b/Jadwal Kuliah.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Zefanya\Dokumen\Kuliah\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361BD04C-B992-40DF-8224-B9C790DC382B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD84777D-7F2C-46C0-B2FE-C1F92FD5CBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{E5D4EB63-BC32-484D-AEFA-16FF28B60A9B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>Senin</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Stupen - MAD LearningX                                      14:00 - Selesai (Zoom)</t>
   </si>
   <si>
-    <t>Stupen - MAD LearningX                                      08:30 - Selesai (Zoom)</t>
-  </si>
-  <si>
     <t>Aslab - Praktikum Database  A                                         10.40 - 12.40 (LIK)</t>
   </si>
   <si>
@@ -244,7 +241,13 @@
     <t>Jadwal Kuliah Semester 5</t>
   </si>
   <si>
-    <t>Stupen - MAD LearningX                                            ?? - ??  (Zoom)</t>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Stupen - MAD LearningX                                            14.00 - Selesai (Zoom)</t>
+  </si>
+  <si>
+    <t>Stupen - MAD LearningX                                      08:30 - Selesai (Zoom) Done</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1716,7 @@
   <dimension ref="C1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C2" sqref="C2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1729,7 +1732,7 @@
     <row r="1" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C2" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="50"/>
       <c r="E2" s="50"/>
@@ -1755,19 +1758,19 @@
     </row>
     <row r="4" spans="3:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="43" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1776,7 +1779,7 @@
       </c>
       <c r="D5" s="39"/>
       <c r="E5" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" s="38"/>
       <c r="G5" s="36"/>
@@ -1808,6 +1811,9 @@
     <row r="10" spans="3:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="8" t="s">
         <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="3:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>